<commit_message>
- Vorlagen Projektstatusbericht verschoben und umbenannt. - Zeittabellen vereinheitlicht
</commit_message>
<xml_diff>
--- a/documents/projectmanagement/Zeitmanagement/Artur.xlsx
+++ b/documents/projectmanagement/Zeitmanagement/Artur.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -18,9 +18,26 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Tätigkeit</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>Dauer (in h)</t>
+  </si>
+  <si>
+    <t>Ort des Dokuments (Falls vorhanden)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +45,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,15 +74,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Akzent5" xfId="1" builtinId="45"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -331,12 +379,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>